<commit_message>
added fast api boiler plate code
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVAM ARORA\IdeaProjects\acad-backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE38334-B5C8-4C7A-A1BB-621A3CA8172E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B861168F-7543-479A-8B62-D5002ECD83FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>task_id</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>Create requirements.txt for the project</t>
+  </si>
+  <si>
+    <t>Setup fast api</t>
+  </si>
+  <si>
+    <t>Create a dummy end point using fast api</t>
+  </si>
+  <si>
+    <t>Setup swagger page</t>
+  </si>
+  <si>
+    <t>Setup swagger page for endpoints</t>
   </si>
 </sst>
 </file>
@@ -369,16 +381,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D2:D3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -424,6 +436,34 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added requirements.txt for dependencies
</commit_message>
<xml_diff>
--- a/docs/task-list.xlsx
+++ b/docs/task-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHIVAM ARORA\IdeaProjects\acad-backend\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B861168F-7543-479A-8B62-D5002ECD83FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34242126-D373-4D27-925A-D67CCE5C69CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>task_id</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Setup swagger page for endpoints</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -384,7 +390,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,7 +439,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -447,7 +453,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>